<commit_message>
fix for uln2003 and other issues
</commit_message>
<xml_diff>
--- a/Compile Sizes.xlsx
+++ b/Compile Sizes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\myFiles\myGitHub\myFP2EFirmware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B5FCC9-E5FD-4233-BCE3-F351D71F14D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7623A754-6192-4328-BFAF-5119DA88BFCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="54">
   <si>
     <t>Program Size</t>
   </si>
@@ -94,97 +94,107 @@
   </si>
   <si>
     <t>JOYSTICK1</t>
+  </si>
+  <si>
+    <t>PUSHBUTTONS !JOYSTICK1</t>
+  </si>
+  <si>
+    <t>JOYSTICK1 !PUSHBUTTONS</t>
+  </si>
+  <si>
+    <t>MSHANDLEROOT</t>
+  </si>
+  <si>
+    <t>MSBUILDROOT</t>
+  </si>
+  <si>
+    <t>MSSENDROOT</t>
+  </si>
+  <si>
+    <t>WSSENDPRESETS</t>
+  </si>
+  <si>
+    <t>WSBUILDPRESETS</t>
+  </si>
+  <si>
+    <t>WSHANDLEPRESETS</t>
+  </si>
+  <si>
+    <t>WSSENDMOVE</t>
+  </si>
+  <si>
+    <t>WSBUILDMOVE</t>
+  </si>
+  <si>
+    <t>WSHANDLEMOVE</t>
+  </si>
+  <si>
+    <t>WSSENDROOT</t>
+  </si>
+  <si>
+    <t>WSBUILDROOT</t>
+  </si>
+  <si>
+    <t>WSHANDLEROOT</t>
+  </si>
+  <si>
+    <t>ASCOMHANDLESETUP</t>
+  </si>
+  <si>
+    <t>ASCOMHANDLEFOCUSERSETUP</t>
+  </si>
+  <si>
+    <t>ASCOMHANDLEAPIVER</t>
+  </si>
+  <si>
+    <t>ASCOMHANDLEAPIDES</t>
+  </si>
+  <si>
+    <t>ASCOMHANDLEAPICON</t>
+  </si>
+  <si>
+    <t>/management/v1/configureddevices</t>
+  </si>
+  <si>
+    <t>/management/v1/description</t>
+  </si>
+  <si>
+    <t>/management/apiversions</t>
+  </si>
+  <si>
+    <t>/setup/v1/focuser/0/setup</t>
+  </si>
+  <si>
+    <t>/setup</t>
+  </si>
+  <si>
+    <t>ASCOMBUILDSETUP</t>
+  </si>
+  <si>
+    <t>EXECUTION TIMINGS [ESP8266]</t>
+  </si>
+  <si>
+    <t>835494 [ESP32]</t>
+  </si>
+  <si>
+    <t>41064 [ESP32]</t>
+  </si>
+  <si>
+    <t>Program Size ESP32</t>
+  </si>
+  <si>
+    <t>Program Size ESP8266</t>
   </si>
   <si>
     <t>STATIONMODE, WEBSERVER, MANAGEMENTSERVER
 SPLASHSCREEN, SHOWSTARTSCREEN, READWIFICONFIG
-PRO2ESP32DRV8825, OLEDTEXT</t>
-  </si>
-  <si>
-    <t>PUSHBUTTONS !JOYSTICK1</t>
-  </si>
-  <si>
-    <t>JOYSTICK1 !PUSHBUTTONS</t>
-  </si>
-  <si>
-    <t>41056 [ESP32 - 12%]
-35588 [ESP8266 - 43%]</t>
-  </si>
-  <si>
-    <t>MSHANDLEROOT</t>
-  </si>
-  <si>
-    <t>MSBUILDROOT</t>
-  </si>
-  <si>
-    <t>MSSENDROOT</t>
-  </si>
-  <si>
-    <t>WSSENDPRESETS</t>
-  </si>
-  <si>
-    <t>WSBUILDPRESETS</t>
-  </si>
-  <si>
-    <t>WSHANDLEPRESETS</t>
-  </si>
-  <si>
-    <t>WSSENDMOVE</t>
-  </si>
-  <si>
-    <t>WSBUILDMOVE</t>
-  </si>
-  <si>
-    <t>WSHANDLEMOVE</t>
-  </si>
-  <si>
-    <t>WSSENDROOT</t>
-  </si>
-  <si>
-    <t>WSBUILDROOT</t>
-  </si>
-  <si>
-    <t>WSHANDLEROOT</t>
-  </si>
-  <si>
-    <t>ASCOMHANDLESETUP</t>
-  </si>
-  <si>
-    <t>ASCOMHANDLEFOCUSERSETUP</t>
-  </si>
-  <si>
-    <t>ASCOMHANDLEAPIVER</t>
-  </si>
-  <si>
-    <t>ASCOMHANDLEAPIDES</t>
-  </si>
-  <si>
-    <t>ASCOMHANDLEAPICON</t>
-  </si>
-  <si>
-    <t>836634 [ESP32 - 63%]
-361104 [ESP8266 - 34%]</t>
-  </si>
-  <si>
-    <t>/management/v1/configureddevices</t>
-  </si>
-  <si>
-    <t>/management/v1/description</t>
-  </si>
-  <si>
-    <t>/management/apiversions</t>
-  </si>
-  <si>
-    <t>/setup/v1/focuser/0/setup</t>
-  </si>
-  <si>
-    <t>/setup</t>
-  </si>
-  <si>
-    <t>ASCOMBUILDSETUP</t>
-  </si>
-  <si>
-    <t>EXECUTION TIMINGS [ESP8266]</t>
+PRO2ESP32DRV8825/PRO2EULN2003, OLEDTEXT</t>
+  </si>
+  <si>
+    <t>Data Size ESP32</t>
+  </si>
+  <si>
+    <t>Data Size ESP8266</t>
   </si>
 </sst>
 </file>
@@ -220,7 +230,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -233,8 +243,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -386,24 +408,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -423,6 +471,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -435,10 +487,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -719,542 +788,692 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="47.90625" customWidth="1"/>
-    <col min="2" max="5" width="21.6796875" customWidth="1"/>
-    <col min="6" max="6" width="4.7265625" customWidth="1"/>
-    <col min="7" max="7" width="28.40625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="21.6796875" customWidth="1"/>
+    <col min="4" max="4" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.31640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.7265625" customWidth="1"/>
+    <col min="9" max="9" width="28.40625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:9" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="B2" s="19">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="B2" s="20">
         <v>122</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="21">
+      <c r="C2" s="21"/>
+      <c r="D2" s="22">
         <v>121</v>
       </c>
-      <c r="E2" s="20"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A3" s="8"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="21"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A3" s="5"/>
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="44.25" x14ac:dyDescent="0.75">
+      <c r="D3" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="32" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.75">
+        <v>51</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="26">
+        <v>836862</v>
+      </c>
+      <c r="E4" s="31">
+        <v>362208</v>
+      </c>
+      <c r="F4" s="29">
+        <v>41080</v>
+      </c>
+      <c r="G4" s="33">
+        <v>35764</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="2">
-        <v>843878</v>
-      </c>
-      <c r="E5" s="3">
-        <v>41152</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="D5" s="27">
+        <v>844106</v>
+      </c>
+      <c r="E5" s="30">
+        <v>366476</v>
+      </c>
+      <c r="F5" s="28">
+        <v>41176</v>
+      </c>
+      <c r="G5" s="32">
+        <v>36120</v>
+      </c>
+      <c r="I5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="2">
-        <v>843894</v>
-      </c>
-      <c r="E6" s="3">
-        <v>41152</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="D6" s="27">
+        <v>844126</v>
+      </c>
+      <c r="E6" s="30">
+        <v>0</v>
+      </c>
+      <c r="F6" s="28">
+        <v>41176</v>
+      </c>
+      <c r="G6" s="32">
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="4">
-        <v>844054</v>
-      </c>
-      <c r="E7" s="3">
-        <v>41152</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="D7" s="25">
+        <v>844294</v>
+      </c>
+      <c r="E7" s="30">
+        <v>366652</v>
+      </c>
+      <c r="F7" s="28">
+        <v>41176</v>
+      </c>
+      <c r="G7" s="32">
+        <v>36120</v>
+      </c>
+      <c r="I7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="4">
-        <v>844222</v>
-      </c>
-      <c r="E8" s="3">
-        <v>41152</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="D8" s="25">
+        <v>844454</v>
+      </c>
+      <c r="E8" s="30">
+        <v>0</v>
+      </c>
+      <c r="F8" s="28">
+        <v>41176</v>
+      </c>
+      <c r="G8" s="32">
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="4">
-        <v>845602</v>
-      </c>
-      <c r="E9" s="3">
-        <v>41160</v>
-      </c>
-      <c r="G9" t="s">
+      <c r="D9" s="25">
+        <v>845862</v>
+      </c>
+      <c r="E9" s="30">
+        <v>0</v>
+      </c>
+      <c r="F9" s="28">
+        <v>41176</v>
+      </c>
+      <c r="G9" s="32">
+        <v>0</v>
+      </c>
+      <c r="I9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="4">
-        <v>845670</v>
-      </c>
-      <c r="E10" s="3">
-        <v>41160</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="D10" s="25">
+        <v>845926</v>
+      </c>
+      <c r="E10" s="30">
+        <v>0</v>
+      </c>
+      <c r="F10" s="28">
+        <v>41168</v>
+      </c>
+      <c r="G10" s="32">
+        <v>0</v>
+      </c>
+      <c r="I10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="4">
-        <v>910702</v>
-      </c>
-      <c r="E11" s="3">
-        <v>41760</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="D11" s="25">
+        <v>909338</v>
+      </c>
+      <c r="E11" s="30">
+        <v>0</v>
+      </c>
+      <c r="F11" s="28">
+        <v>41768</v>
+      </c>
+      <c r="G11" s="32">
+        <v>0</v>
+      </c>
+      <c r="I11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
         <v>3</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="4">
-        <v>957558</v>
-      </c>
-      <c r="E12" s="3">
-        <v>45920</v>
-      </c>
-      <c r="G12" t="s">
+      <c r="D12" s="25">
+        <v>956210</v>
+      </c>
+      <c r="E12" s="30">
+        <v>403956</v>
+      </c>
+      <c r="F12" s="28">
+        <v>45928</v>
+      </c>
+      <c r="G12" s="32">
+        <v>36688</v>
+      </c>
+      <c r="I12" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="4">
-        <v>991722</v>
-      </c>
-      <c r="E13" s="3">
-        <v>46320</v>
-      </c>
-      <c r="G13" t="s">
+      <c r="D13" s="25">
+        <v>988094</v>
+      </c>
+      <c r="E13" s="30">
+        <v>420812</v>
+      </c>
+      <c r="F13" s="28">
+        <v>46336</v>
+      </c>
+      <c r="G13" s="32">
+        <v>41072</v>
+      </c>
+      <c r="I13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A14" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="3"/>
-      <c r="D14" s="4">
-        <v>992514</v>
-      </c>
-      <c r="E14" s="3">
-        <v>46336</v>
-      </c>
-      <c r="G14" t="s">
+      <c r="D14" s="25">
+        <v>988910</v>
+      </c>
+      <c r="E14" s="30">
+        <v>421280</v>
+      </c>
+      <c r="F14" s="28">
+        <v>46344</v>
+      </c>
+      <c r="G14" s="32">
+        <v>41244</v>
+      </c>
+      <c r="I14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A15" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="4">
-        <v>1166322</v>
-      </c>
-      <c r="E15" s="3">
-        <v>46984</v>
-      </c>
-      <c r="G15" t="s">
+      <c r="D15" s="25">
+        <v>1162766</v>
+      </c>
+      <c r="E15" s="30">
+        <v>429624</v>
+      </c>
+      <c r="F15" s="28">
+        <v>46992</v>
+      </c>
+      <c r="G15" s="32">
+        <v>42116</v>
+      </c>
+      <c r="I15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A16" t="s">
         <v>2</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="3"/>
-      <c r="D16" s="4">
-        <v>1186630</v>
-      </c>
-      <c r="E16" s="3">
-        <v>47120</v>
-      </c>
-      <c r="G16" t="s">
+      <c r="D16" s="25">
+        <v>1184094</v>
+      </c>
+      <c r="E16" s="30">
+        <v>444916</v>
+      </c>
+      <c r="F16" s="28">
+        <v>47128</v>
+      </c>
+      <c r="G16" s="32">
+        <v>45208</v>
+      </c>
+      <c r="I16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A17" s="8" t="s">
+    <row r="17" spans="1:7" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="A17" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="13"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="15">
+      <c r="B17" s="10"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="12">
         <v>90</v>
       </c>
-      <c r="E17" s="11">
+      <c r="E17" s="24">
+        <v>42</v>
+      </c>
+      <c r="F17" s="24">
         <v>14</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A19" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="G17" s="8">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A19" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A20" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9">
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6">
         <v>1</v>
       </c>
-      <c r="E20" s="9"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A21" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A22" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="24">
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="17">
         <v>1292</v>
       </c>
-      <c r="E22" s="9"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="9"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="6"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="6"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="17">
+        <v>91</v>
+      </c>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6">
+        <v>67</v>
+      </c>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A26" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9">
-        <v>91</v>
-      </c>
-      <c r="E24" s="9"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A25" t="s">
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="15">
+        <v>245</v>
+      </c>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="6"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="17">
+        <v>120</v>
+      </c>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="6"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6">
+        <v>29</v>
+      </c>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6">
+        <v>59</v>
+      </c>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6">
+        <v>75</v>
+      </c>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6">
+        <v>40</v>
+      </c>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6">
+        <v>74</v>
+      </c>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A33" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7">
+        <v>16</v>
+      </c>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A34" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9">
-        <v>67</v>
-      </c>
-      <c r="E25" s="9"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A26" t="s">
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7">
+        <v>26</v>
+      </c>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="I34" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A35" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="22">
-        <v>245</v>
-      </c>
-      <c r="E26" s="9"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A27" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="24">
-        <v>120</v>
-      </c>
-      <c r="E27" s="9"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A28" t="s">
-        <v>32</v>
-      </c>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9">
-        <v>29</v>
-      </c>
-      <c r="E28" s="9"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A29" t="s">
-        <v>33</v>
-      </c>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9">
-        <v>59</v>
-      </c>
-      <c r="E29" s="9"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A30" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9">
-        <v>75</v>
-      </c>
-      <c r="E30" s="9"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A31" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9">
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7">
+        <v>38</v>
+      </c>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="I35" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A36" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7">
+        <v>2</v>
+      </c>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="I36" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A37" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7">
+        <v>3</v>
+      </c>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="I37" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A38" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7">
+        <v>2</v>
+      </c>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="I38" t="s">
         <v>40</v>
       </c>
-      <c r="E31" s="9"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A32" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9">
-        <v>74</v>
-      </c>
-      <c r="E32" s="9"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A33" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10">
-        <v>16</v>
-      </c>
-      <c r="E33" s="10"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A34" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10">
-        <v>26</v>
-      </c>
-      <c r="E34" s="10"/>
-      <c r="G34" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A35" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10">
-        <v>38</v>
-      </c>
-      <c r="E35" s="10"/>
-      <c r="G35" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A36" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B36" s="10"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10">
-        <v>2</v>
-      </c>
-      <c r="E36" s="10"/>
-      <c r="G36" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A37" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="B37" s="10"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10">
-        <v>3</v>
-      </c>
-      <c r="E37" s="10"/>
-      <c r="G37" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A38" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B38" s="10"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10">
-        <v>2</v>
-      </c>
-      <c r="E38" s="10"/>
-      <c r="G38" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A39" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B39" s="10"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="23">
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A39" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="16">
         <v>157</v>
       </c>
-      <c r="E39" s="10"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A40" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B40" s="10"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="10">
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="7"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A40" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7">
         <v>56</v>
       </c>
-      <c r="E40" s="10"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A41" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B41" s="10"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10">
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A41" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7">
         <v>61</v>
       </c>
-      <c r="E41" s="10"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="B42" s="12" t="s">
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="B42" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C42" s="12" t="s">
+      <c r="C42" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D42" s="12" t="s">
+      <c r="D42" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E42" s="12" t="s">
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1262,8 +1481,8 @@
   <mergeCells count="4">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="D2:G2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
hpsw fixes, ascom root page fixes
</commit_message>
<xml_diff>
--- a/Compile Sizes.xlsx
+++ b/Compile Sizes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\myFiles\myArduino\myFocuserPro2ESP\Firmware myFP2ESP\myFP2EFirmware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\myFiles\myGitHub\myFP2EFirmware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871C93BA-6462-415B-A00D-B9493520CE04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{473ED180-6479-4FA3-9671-D38E05D49B5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="80">
   <si>
     <t>Program Size</t>
   </si>
@@ -250,23 +250,25 @@
   </si>
   <si>
     <t>125 : ESP32</t>
+  </si>
+  <si>
+    <t>INFRAREDREMOTE [NO PB, NO JY]</t>
+  </si>
+  <si>
+    <t>ESP32 Core 1.0.4</t>
+  </si>
+  <si>
+    <t>ArduinJSON 6.16.1</t>
+  </si>
+  <si>
+    <t>130 : ESP32</t>
   </si>
   <si>
     <t>ACCESSPOINT
 MANAGEMENTSERVER
 PRO2ESP32DRV8825
-TIMEDTESTS
 HEAPDEBUG OFF
 TIMEDTESTS OFF</t>
-  </si>
-  <si>
-    <t>INFRAREDREMOTE [NO PB, NO JY]</t>
-  </si>
-  <si>
-    <t>ESP32 Core 1.0.4</t>
-  </si>
-  <si>
-    <t>ArduinJSON 6.16.1</t>
   </si>
 </sst>
 </file>
@@ -302,7 +304,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -345,6 +347,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -498,7 +506,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -561,6 +569,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -841,123 +854,135 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K57"/>
+  <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="36.2265625" customWidth="1"/>
-    <col min="2" max="5" width="14.6796875" customWidth="1"/>
-    <col min="6" max="6" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.6796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.7265625" customWidth="1"/>
-    <col min="11" max="11" width="28.40625" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="14.6796875" customWidth="1"/>
+    <col min="8" max="8" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.6796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.7265625" customWidth="1"/>
+    <col min="13" max="13" width="28.40625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="1" spans="1:13" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="G1" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="H1" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="I1" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A2" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C2" s="38"/>
       <c r="D2" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" s="38"/>
+      <c r="F2" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="E2" s="38"/>
-      <c r="F2" s="37">
+      <c r="G2" s="38"/>
+      <c r="H2" s="37">
         <v>121</v>
       </c>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="38"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="38"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A3" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="15" t="s">
+      <c r="D3" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="G3" s="31" t="s">
+      <c r="I3" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="H3" s="32" t="s">
+      <c r="J3" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="I3" s="15" t="s">
+      <c r="K3" s="41" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="88.5" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:13" ht="73.75" x14ac:dyDescent="0.75">
       <c r="A4" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B4" s="13">
+        <v>893982</v>
+      </c>
+      <c r="C4" s="16">
+        <v>40896</v>
+      </c>
+      <c r="D4" s="13">
         <v>898294</v>
-      </c>
-      <c r="C4" s="16">
-        <v>41000</v>
-      </c>
-      <c r="D4" s="13">
-        <v>40872</v>
       </c>
       <c r="E4" s="16">
         <v>41000</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="13"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="13">
         <v>836862</v>
       </c>
-      <c r="G4" s="33">
+      <c r="I4" s="33">
         <v>362208</v>
       </c>
-      <c r="H4" s="34">
+      <c r="J4" s="34">
         <v>41080</v>
       </c>
-      <c r="I4" s="16">
+      <c r="K4" s="16">
         <v>35764</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -974,22 +999,28 @@
         <v>0</v>
       </c>
       <c r="F5" s="14">
+        <v>0</v>
+      </c>
+      <c r="G5" s="15">
+        <v>0</v>
+      </c>
+      <c r="H5" s="14">
         <v>844106</v>
       </c>
-      <c r="G5" s="31">
+      <c r="I5" s="31">
         <v>366476</v>
       </c>
-      <c r="H5" s="32">
+      <c r="J5" s="32">
         <v>41176</v>
       </c>
-      <c r="I5" s="15">
+      <c r="K5" s="15">
         <v>36120</v>
       </c>
-      <c r="K5" t="s">
+      <c r="M5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1005,12 +1036,18 @@
       <c r="E6" s="15">
         <v>0</v>
       </c>
-      <c r="F6" s="14"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="15"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="F6" s="14">
+        <v>0</v>
+      </c>
+      <c r="G6" s="15">
+        <v>0</v>
+      </c>
+      <c r="H6" s="14"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="15"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1026,12 +1063,18 @@
       <c r="E7" s="15">
         <v>0</v>
       </c>
-      <c r="F7" s="14"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="15"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="F7" s="14">
+        <v>0</v>
+      </c>
+      <c r="G7" s="15">
+        <v>0</v>
+      </c>
+      <c r="H7" s="14"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="15"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>51</v>
       </c>
@@ -1047,12 +1090,18 @@
       <c r="E8" s="15">
         <v>0</v>
       </c>
-      <c r="F8" s="14"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="15"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="F8" s="14">
+        <v>0</v>
+      </c>
+      <c r="G8" s="15">
+        <v>0</v>
+      </c>
+      <c r="H8" s="14"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="32"/>
+      <c r="K8" s="15"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1068,291 +1117,353 @@
       <c r="E9" s="15">
         <v>0</v>
       </c>
-      <c r="F9" s="14"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="15"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="F9" s="14">
+        <v>0</v>
+      </c>
+      <c r="G9" s="15">
+        <v>0</v>
+      </c>
+      <c r="H9" s="14"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="15"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>52</v>
       </c>
       <c r="B10" s="14">
+        <v>906658</v>
+      </c>
+      <c r="C10" s="15">
+        <v>41720</v>
+      </c>
+      <c r="D10" s="14">
         <v>911758</v>
       </c>
-      <c r="C10" s="15">
+      <c r="E10" s="15">
         <v>41632</v>
       </c>
-      <c r="D10" s="14">
+      <c r="F10" s="14">
         <v>912942</v>
       </c>
-      <c r="E10" s="15">
+      <c r="G10" s="15">
         <v>41768</v>
       </c>
-      <c r="F10" s="14"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="15"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="H10" s="14"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="15"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="14">
+        <v>907226</v>
+      </c>
+      <c r="C11" s="15">
+        <v>41728</v>
+      </c>
+      <c r="D11" s="14">
         <v>912326</v>
       </c>
-      <c r="C11" s="15">
+      <c r="E11" s="15">
         <v>41632</v>
       </c>
-      <c r="D11" s="14">
+      <c r="F11" s="14">
         <v>913106</v>
       </c>
-      <c r="E11" s="15">
+      <c r="G11" s="15">
         <v>41768</v>
       </c>
-      <c r="F11" s="14">
+      <c r="H11" s="14">
         <v>844126</v>
       </c>
-      <c r="G11" s="31">
-        <v>0</v>
-      </c>
-      <c r="H11" s="32">
+      <c r="I11" s="31">
+        <v>0</v>
+      </c>
+      <c r="J11" s="32">
         <v>41176</v>
       </c>
-      <c r="I11" s="15">
-        <v>0</v>
-      </c>
-      <c r="K11" t="s">
+      <c r="K11" s="15">
+        <v>0</v>
+      </c>
+      <c r="M11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
         <v>21</v>
       </c>
       <c r="B12" s="14">
+        <v>907406</v>
+      </c>
+      <c r="C12" s="15">
+        <v>41728</v>
+      </c>
+      <c r="D12" s="14">
         <v>912462</v>
       </c>
-      <c r="C12" s="15">
+      <c r="E12" s="15">
         <v>41632</v>
       </c>
-      <c r="D12" s="14">
+      <c r="F12" s="14">
         <v>913294</v>
       </c>
-      <c r="E12" s="15">
+      <c r="G12" s="15">
         <v>41768</v>
       </c>
-      <c r="F12" s="14">
+      <c r="H12" s="14">
         <v>844454</v>
       </c>
-      <c r="G12" s="31">
-        <v>0</v>
-      </c>
-      <c r="H12" s="32">
+      <c r="I12" s="31">
+        <v>0</v>
+      </c>
+      <c r="J12" s="32">
         <v>41176</v>
       </c>
-      <c r="I12" s="15">
-        <v>0</v>
-      </c>
-      <c r="K12" t="s">
+      <c r="K12" s="15">
+        <v>0</v>
+      </c>
+      <c r="M12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="14">
+        <v>908858</v>
+      </c>
+      <c r="C13" s="15">
+        <v>41736</v>
+      </c>
+      <c r="D13" s="14">
         <v>913894</v>
       </c>
-      <c r="C13" s="15">
+      <c r="E13" s="15">
         <v>41640</v>
       </c>
-      <c r="D13" s="14">
+      <c r="F13" s="14">
         <v>914714</v>
       </c>
-      <c r="E13" s="15">
+      <c r="G13" s="15">
         <v>41776</v>
       </c>
-      <c r="F13" s="14">
+      <c r="H13" s="14">
         <v>845862</v>
       </c>
-      <c r="G13" s="31">
-        <v>0</v>
-      </c>
-      <c r="H13" s="32">
+      <c r="I13" s="31">
+        <v>0</v>
+      </c>
+      <c r="J13" s="32">
         <v>41176</v>
       </c>
-      <c r="I13" s="15">
-        <v>0</v>
-      </c>
-      <c r="K13" t="s">
+      <c r="K13" s="15">
+        <v>0</v>
+      </c>
+      <c r="M13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B14" s="14">
+        <v>913538</v>
+      </c>
+      <c r="C14" s="15">
+        <v>41864</v>
+      </c>
+      <c r="D14" s="14">
         <v>918338</v>
       </c>
-      <c r="C14" s="15">
+      <c r="E14" s="15">
         <v>41776</v>
       </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="14">
+      <c r="F14" s="14"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="14">
         <v>909338</v>
       </c>
-      <c r="G14" s="31">
-        <v>0</v>
-      </c>
-      <c r="H14" s="32">
+      <c r="I14" s="31">
+        <v>0</v>
+      </c>
+      <c r="J14" s="32">
         <v>41768</v>
       </c>
-      <c r="I14" s="15">
-        <v>0</v>
-      </c>
-      <c r="K14" t="s">
+      <c r="K14" s="15">
+        <v>0</v>
+      </c>
+      <c r="M14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A15" t="s">
         <v>66</v>
       </c>
       <c r="B15" s="14">
+        <v>914970</v>
+      </c>
+      <c r="C15" s="15">
+        <v>41880</v>
+      </c>
+      <c r="D15" s="14">
         <v>919742</v>
       </c>
-      <c r="C15" s="15">
+      <c r="E15" s="15">
         <v>41776</v>
       </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="15"/>
       <c r="F15" s="14"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="15"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="G15" s="15"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="15"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A16" t="s">
         <v>67</v>
       </c>
       <c r="B16" s="14">
+        <v>960466</v>
+      </c>
+      <c r="C16" s="15">
+        <v>45712</v>
+      </c>
+      <c r="D16" s="14">
         <v>965314</v>
       </c>
-      <c r="C16" s="15">
+      <c r="E16" s="15">
         <v>45616</v>
       </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="14">
+      <c r="F16" s="14"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="14">
         <v>956210</v>
       </c>
-      <c r="G16" s="31">
+      <c r="I16" s="31">
         <v>403956</v>
       </c>
-      <c r="H16" s="32">
+      <c r="J16" s="32">
         <v>45928</v>
       </c>
-      <c r="I16" s="15">
+      <c r="K16" s="15">
         <v>36688</v>
       </c>
-      <c r="K16" t="s">
+      <c r="M16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A17" t="s">
         <v>68</v>
       </c>
       <c r="B17" s="14">
+        <v>961286</v>
+      </c>
+      <c r="C17" s="15">
+        <v>45720</v>
+      </c>
+      <c r="D17" s="14">
         <v>966130</v>
       </c>
-      <c r="C17" s="15">
+      <c r="E17" s="15">
         <v>45624</v>
       </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="14">
+      <c r="F17" s="14"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="14">
         <v>988910</v>
       </c>
-      <c r="G17" s="31">
+      <c r="I17" s="31">
         <v>421280</v>
       </c>
-      <c r="H17" s="32">
+      <c r="J17" s="32">
         <v>46344</v>
       </c>
-      <c r="I17" s="15">
+      <c r="K17" s="15">
         <v>41244</v>
       </c>
-      <c r="K17" t="s">
+      <c r="M17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A18" t="s">
         <v>69</v>
       </c>
       <c r="B18" s="14">
+        <v>1135206</v>
+      </c>
+      <c r="C18" s="15">
+        <v>46376</v>
+      </c>
+      <c r="D18" s="14">
         <v>1139754</v>
       </c>
-      <c r="C18" s="15">
+      <c r="E18" s="15">
         <v>46272</v>
       </c>
-      <c r="D18" s="14"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="14">
+      <c r="F18" s="14"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="14">
         <v>1162766</v>
       </c>
-      <c r="G18" s="31">
+      <c r="I18" s="31">
         <v>429624</v>
       </c>
-      <c r="H18" s="32">
+      <c r="J18" s="32">
         <v>46992</v>
       </c>
-      <c r="I18" s="15">
+      <c r="K18" s="15">
         <v>42116</v>
       </c>
-      <c r="K18" t="s">
+      <c r="M18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A19" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="14">
+      <c r="B19" s="14"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="14">
         <v>1160594</v>
       </c>
-      <c r="C19" s="15">
+      <c r="E19" s="15">
         <v>46272</v>
       </c>
-      <c r="D19" s="14"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="14">
+      <c r="F19" s="14"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="14">
         <v>1184094</v>
       </c>
-      <c r="G19" s="31">
+      <c r="I19" s="31">
         <v>444916</v>
       </c>
-      <c r="H19" s="32">
+      <c r="J19" s="32">
         <v>47128</v>
       </c>
-      <c r="I19" s="15">
+      <c r="K19" s="15">
         <v>45208</v>
       </c>
-      <c r="K19" t="s">
+      <c r="M19" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="20" spans="1:13" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A20" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B20" s="20">
-        <v>0.88</v>
+        <v>0.86</v>
       </c>
       <c r="C20" s="21">
         <v>0.14000000000000001</v>
@@ -1363,20 +1474,26 @@
       <c r="E20" s="21">
         <v>0.14000000000000001</v>
       </c>
-      <c r="F20" s="35">
+      <c r="F20" s="20">
+        <v>0.88</v>
+      </c>
+      <c r="G20" s="21">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="H20" s="35">
         <v>90</v>
       </c>
-      <c r="G20" s="36">
+      <c r="I20" s="36">
         <v>42</v>
       </c>
-      <c r="H20" s="36">
+      <c r="J20" s="36">
         <v>14</v>
       </c>
-      <c r="I20" s="6">
+      <c r="K20" s="6">
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A22" s="3" t="s">
         <v>46</v>
       </c>
@@ -1388,25 +1505,29 @@
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A23" t="s">
         <v>5</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
-      <c r="D23" s="28">
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="28">
         <v>1</v>
       </c>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4">
+      <c r="G23" s="4"/>
+      <c r="H23" s="4">
         <v>1</v>
       </c>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
       <c r="I23" s="4"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -1418,557 +1539,681 @@
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A25" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="4"/>
+      <c r="B25" s="17">
+        <v>1301</v>
+      </c>
       <c r="C25" s="4"/>
-      <c r="D25" s="17">
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="17">
         <v>662</v>
       </c>
-      <c r="E25" s="4"/>
-      <c r="F25" s="11">
+      <c r="G25" s="4"/>
+      <c r="H25" s="11">
         <v>1292</v>
       </c>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="4"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="4"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.75">
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
       <c r="H26" s="12"/>
-      <c r="I26" s="4"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="4"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A27" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="28">
+      <c r="B27" s="17">
+        <v>92</v>
+      </c>
+      <c r="C27" s="4"/>
+      <c r="D27" s="28">
         <v>72</v>
-      </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="11">
-        <v>172</v>
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="11">
+        <v>172</v>
+      </c>
+      <c r="G27" s="4"/>
+      <c r="H27" s="11">
         <v>91</v>
       </c>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="4"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="4"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A28" t="s">
         <v>33</v>
       </c>
       <c r="B28" s="28">
-        <v>59</v>
+        <v>117</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="28">
         <v>59</v>
       </c>
       <c r="E28" s="4"/>
-      <c r="F28" s="4">
+      <c r="F28" s="28">
+        <v>59</v>
+      </c>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4">
         <v>67</v>
       </c>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="4"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="4"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A29" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="4"/>
+      <c r="B29" s="17">
+        <v>96</v>
+      </c>
       <c r="C29" s="4"/>
-      <c r="D29" s="4">
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4">
         <v>79</v>
       </c>
-      <c r="E29" s="4"/>
-      <c r="F29" s="9">
+      <c r="G29" s="4"/>
+      <c r="H29" s="9">
         <v>245</v>
       </c>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="4"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
+      <c r="K29" s="4"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A30" t="s">
         <v>29</v>
       </c>
       <c r="B30" s="11">
+        <v>109</v>
+      </c>
+      <c r="C30" s="4"/>
+      <c r="D30" s="11">
         <v>104</v>
       </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="28">
+      <c r="E30" s="4"/>
+      <c r="F30" s="28">
         <v>63</v>
       </c>
-      <c r="E30" s="4"/>
-      <c r="F30" s="11">
+      <c r="G30" s="4"/>
+      <c r="H30" s="11">
         <v>120</v>
       </c>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="4"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="4"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A31" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="17">
+      <c r="B31" s="44">
+        <v>52</v>
+      </c>
+      <c r="C31" s="4"/>
+      <c r="D31" s="17">
         <v>92</v>
       </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="28">
+      <c r="E31" s="4"/>
+      <c r="F31" s="28">
         <v>50</v>
       </c>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4">
+      <c r="G31" s="4"/>
+      <c r="H31" s="4">
         <v>29</v>
       </c>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
       <c r="I31" s="4"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A32" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="4"/>
+      <c r="B32" s="11">
+        <v>178</v>
+      </c>
       <c r="C32" s="4"/>
-      <c r="D32" s="28">
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="28">
         <v>73</v>
       </c>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4">
+      <c r="G32" s="4"/>
+      <c r="H32" s="4">
         <v>59</v>
       </c>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
       <c r="I32" s="4"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A33" t="s">
         <v>26</v>
       </c>
       <c r="B33" s="17">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C33" s="4"/>
       <c r="D33" s="17">
+        <v>83</v>
+      </c>
+      <c r="E33" s="4"/>
+      <c r="F33" s="17">
         <v>80</v>
       </c>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4">
+      <c r="G33" s="4"/>
+      <c r="H33" s="4">
         <v>75</v>
       </c>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
       <c r="I33" s="4"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="J33" s="4"/>
+      <c r="K33" s="4"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A34" t="s">
         <v>27</v>
       </c>
-      <c r="B34" s="28">
-        <v>71</v>
+      <c r="B34" s="44">
+        <v>70</v>
       </c>
       <c r="C34" s="4"/>
       <c r="D34" s="28">
         <v>71</v>
       </c>
       <c r="E34" s="4"/>
-      <c r="F34" s="4">
+      <c r="F34" s="28">
+        <v>71</v>
+      </c>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4">
         <v>40</v>
       </c>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
       <c r="I34" s="4"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="J34" s="4"/>
+      <c r="K34" s="4"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A35" t="s">
         <v>28</v>
       </c>
-      <c r="B35" s="4"/>
+      <c r="B35" s="17">
+        <v>96</v>
+      </c>
       <c r="C35" s="4"/>
-      <c r="D35" s="17">
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="17">
         <v>92</v>
       </c>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4">
+      <c r="G35" s="4"/>
+      <c r="H35" s="4">
         <v>74</v>
       </c>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
       <c r="I35" s="4"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A36" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B36" s="5"/>
+      <c r="B36" s="5">
+        <v>36</v>
+      </c>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
-      <c r="F36" s="5">
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5">
         <v>16</v>
       </c>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
       <c r="I36" s="5"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A37" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B37" s="29">
-        <v>54</v>
+      <c r="B37" s="5">
+        <v>35</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="29">
+        <v>54</v>
+      </c>
+      <c r="E37" s="5"/>
+      <c r="F37" s="29">
         <v>57</v>
       </c>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5">
+      <c r="G37" s="5"/>
+      <c r="H37" s="5">
         <v>26</v>
       </c>
-      <c r="G37" s="5"/>
-      <c r="H37" s="5"/>
       <c r="I37" s="5"/>
-      <c r="K37" t="s">
+      <c r="J37" s="5"/>
+      <c r="K37" s="5"/>
+      <c r="M37" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A38" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B38" s="29">
-        <v>29</v>
+      <c r="B38" s="5">
+        <v>35</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="29">
+        <v>29</v>
+      </c>
+      <c r="E38" s="5"/>
+      <c r="F38" s="29">
         <v>68</v>
       </c>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5">
+      <c r="G38" s="5"/>
+      <c r="H38" s="5">
         <v>38</v>
       </c>
-      <c r="G38" s="5"/>
-      <c r="H38" s="5"/>
       <c r="I38" s="5"/>
-      <c r="K38" t="s">
+      <c r="J38" s="5"/>
+      <c r="K38" s="5"/>
+      <c r="M38" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A39" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B39" s="5"/>
+      <c r="B39" s="5">
+        <v>3</v>
+      </c>
       <c r="C39" s="5"/>
-      <c r="D39" s="29">
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="29">
         <v>2</v>
       </c>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5">
+      <c r="G39" s="5"/>
+      <c r="H39" s="5">
         <v>2</v>
       </c>
-      <c r="G39" s="5"/>
-      <c r="H39" s="5"/>
       <c r="I39" s="5"/>
-      <c r="K39" t="s">
+      <c r="J39" s="5"/>
+      <c r="K39" s="5"/>
+      <c r="M39" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A40" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B40" s="30"/>
+      <c r="B40" s="30">
+        <v>3</v>
+      </c>
       <c r="C40" s="30"/>
-      <c r="D40" s="29">
+      <c r="D40" s="30"/>
+      <c r="E40" s="30"/>
+      <c r="F40" s="29">
         <v>3</v>
       </c>
-      <c r="E40" s="5"/>
-      <c r="F40" s="5">
+      <c r="G40" s="5"/>
+      <c r="H40" s="5">
         <v>3</v>
       </c>
-      <c r="G40" s="5"/>
-      <c r="H40" s="5"/>
       <c r="I40" s="5"/>
-      <c r="K40" t="s">
+      <c r="J40" s="5"/>
+      <c r="K40" s="5"/>
+      <c r="M40" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A41" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B41" s="5"/>
+      <c r="B41" s="5">
+        <v>3</v>
+      </c>
       <c r="C41" s="5"/>
-      <c r="D41" s="29">
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="29">
         <v>66</v>
       </c>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5">
+      <c r="G41" s="5"/>
+      <c r="H41" s="5">
         <v>2</v>
       </c>
-      <c r="G41" s="5"/>
-      <c r="H41" s="5"/>
       <c r="I41" s="5"/>
-      <c r="K41" t="s">
+      <c r="J41" s="5"/>
+      <c r="K41" s="5"/>
+      <c r="M41" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A42" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B42" s="18">
-        <v>83</v>
+      <c r="B42" s="28">
+        <v>48</v>
       </c>
       <c r="C42" s="5"/>
       <c r="D42" s="18">
         <v>83</v>
       </c>
       <c r="E42" s="5"/>
-      <c r="F42" s="10">
+      <c r="F42" s="18">
+        <v>83</v>
+      </c>
+      <c r="G42" s="5"/>
+      <c r="H42" s="10">
         <v>157</v>
       </c>
-      <c r="G42" s="10"/>
-      <c r="H42" s="10"/>
-      <c r="I42" s="5"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="I42" s="10"/>
+      <c r="J42" s="10"/>
+      <c r="K42" s="5"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A43" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B43" s="29">
-        <v>72</v>
+      <c r="B43" s="28">
+        <v>33</v>
       </c>
       <c r="C43" s="5"/>
       <c r="D43" s="29">
+        <v>72</v>
+      </c>
+      <c r="E43" s="5"/>
+      <c r="F43" s="29">
         <v>70</v>
       </c>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5">
+      <c r="G43" s="5"/>
+      <c r="H43" s="5">
         <v>56</v>
       </c>
-      <c r="G43" s="5"/>
-      <c r="H43" s="5"/>
       <c r="I43" s="5"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="J43" s="5"/>
+      <c r="K43" s="5"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A44" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B44" s="5"/>
+      <c r="B44" s="28">
+        <v>96</v>
+      </c>
       <c r="C44" s="5"/>
-      <c r="D44" s="18">
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="18">
         <v>93</v>
       </c>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5">
+      <c r="G44" s="5"/>
+      <c r="H44" s="5">
         <v>61</v>
       </c>
-      <c r="G44" s="5"/>
-      <c r="H44" s="5"/>
       <c r="I44" s="5"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="J44" s="5"/>
+      <c r="K44" s="5"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A45" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B45" s="29">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="C45" s="5"/>
       <c r="D45" s="29">
+        <v>53</v>
+      </c>
+      <c r="E45" s="5"/>
+      <c r="F45" s="29">
         <v>56</v>
       </c>
-      <c r="E45" s="5"/>
-      <c r="F45" s="5"/>
       <c r="G45" s="5"/>
       <c r="H45" s="5"/>
       <c r="I45" s="5"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="J45" s="5"/>
+      <c r="K45" s="5"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A46" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B46" s="29">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C46" s="5"/>
       <c r="D46" s="29">
+        <v>41</v>
+      </c>
+      <c r="E46" s="5"/>
+      <c r="F46" s="29">
         <v>44</v>
       </c>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
       <c r="G46" s="5"/>
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="J46" s="5"/>
+      <c r="K46" s="5"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A47" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B47" s="29">
+        <v>61</v>
+      </c>
+      <c r="C47" s="5"/>
+      <c r="D47" s="29">
         <v>77</v>
       </c>
-      <c r="C47" s="5"/>
-      <c r="D47" s="19">
+      <c r="E47" s="5"/>
+      <c r="F47" s="19">
         <v>105</v>
       </c>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
       <c r="G47" s="5"/>
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="J47" s="5"/>
+      <c r="K47" s="5"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A48" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B48" s="29">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C48" s="5"/>
       <c r="D48" s="29">
         <v>38</v>
       </c>
       <c r="E48" s="5"/>
-      <c r="F48" s="5"/>
+      <c r="F48" s="29">
+        <v>38</v>
+      </c>
       <c r="G48" s="5"/>
       <c r="H48" s="5"/>
       <c r="I48" s="5"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J48" s="5"/>
+      <c r="K48" s="5"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A49" s="2" t="s">
         <v>58</v>
       </c>
       <c r="B49" s="29">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C49" s="5"/>
       <c r="D49" s="29">
         <v>26</v>
       </c>
       <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
+      <c r="F49" s="29">
+        <v>26</v>
+      </c>
       <c r="G49" s="5"/>
       <c r="H49" s="5"/>
       <c r="I49" s="5"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J49" s="5"/>
+      <c r="K49" s="5"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A50" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B50" s="5"/>
+      <c r="B50" s="29">
+        <v>52</v>
+      </c>
       <c r="C50" s="5"/>
-      <c r="D50" s="29">
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="29">
         <v>47</v>
       </c>
-      <c r="E50" s="5"/>
-      <c r="F50" s="5"/>
       <c r="G50" s="5"/>
       <c r="H50" s="5"/>
       <c r="I50" s="5"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J50" s="5"/>
+      <c r="K50" s="5"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A51" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B51" s="29">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C51" s="5"/>
       <c r="D51" s="29">
         <v>39</v>
       </c>
       <c r="E51" s="5"/>
-      <c r="F51" s="5"/>
+      <c r="F51" s="29">
+        <v>39</v>
+      </c>
       <c r="G51" s="5"/>
       <c r="H51" s="5"/>
       <c r="I51" s="5"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J51" s="5"/>
+      <c r="K51" s="5"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A52" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B52" s="29">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C52" s="5"/>
       <c r="D52" s="29">
         <v>27</v>
       </c>
       <c r="E52" s="5"/>
-      <c r="F52" s="5"/>
+      <c r="F52" s="29">
+        <v>27</v>
+      </c>
       <c r="G52" s="5"/>
       <c r="H52" s="5"/>
       <c r="I52" s="5"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J52" s="5"/>
+      <c r="K52" s="5"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A53" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B53" s="5"/>
+      <c r="B53" s="29">
+        <v>53</v>
+      </c>
       <c r="C53" s="5"/>
-      <c r="D53" s="29">
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="29">
         <v>48</v>
       </c>
-      <c r="E53" s="5"/>
-      <c r="F53" s="5"/>
       <c r="G53" s="5"/>
       <c r="H53" s="5"/>
       <c r="I53" s="5"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J53" s="5"/>
+      <c r="K53" s="5"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A54" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B54" s="29">
+        <v>63</v>
+      </c>
+      <c r="C54" s="5"/>
+      <c r="D54" s="29">
         <v>58</v>
       </c>
-      <c r="C54" s="5"/>
-      <c r="D54" s="18">
+      <c r="E54" s="5"/>
+      <c r="F54" s="18">
         <v>86</v>
       </c>
-      <c r="E54" s="5"/>
-      <c r="F54" s="5"/>
       <c r="G54" s="5"/>
       <c r="H54" s="5"/>
       <c r="I54" s="5"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J54" s="5"/>
+      <c r="K54" s="5"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A55" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B55" s="29">
+        <v>49</v>
+      </c>
+      <c r="C55" s="5"/>
+      <c r="D55" s="29">
         <v>46</v>
       </c>
-      <c r="C55" s="5"/>
-      <c r="D55" s="18">
+      <c r="E55" s="5"/>
+      <c r="F55" s="18">
         <v>98</v>
       </c>
-      <c r="E55" s="5"/>
-      <c r="F55" s="5"/>
       <c r="G55" s="5"/>
       <c r="H55" s="5"/>
       <c r="I55" s="5"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J55" s="5"/>
+      <c r="K55" s="5"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A56" s="2" t="s">
         <v>65</v>
       </c>
@@ -1980,18 +2225,20 @@
         <v>0</v>
       </c>
       <c r="E56" s="5"/>
-      <c r="F56" s="5"/>
+      <c r="F56" s="5">
+        <v>0</v>
+      </c>
       <c r="G56" s="5"/>
       <c r="H56" s="5"/>
       <c r="I56" s="5"/>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J56" s="5"/>
+      <c r="K56" s="5"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.75">
       <c r="B57" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C57" s="7" t="s">
-        <v>9</v>
-      </c>
+      <c r="C57" s="4"/>
       <c r="D57" s="7" t="s">
         <v>8</v>
       </c>
@@ -2001,16 +2248,23 @@
       <c r="F57" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G57" s="7"/>
-      <c r="H57" s="7"/>
-      <c r="I57" s="7" t="s">
+      <c r="G57" s="7" t="s">
         <v>9</v>
       </c>
+      <c r="H57" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I57" s="7"/>
+      <c r="J57" s="7"/>
+      <c r="K57" s="7" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:K2"/>
     <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:I2"/>
     <mergeCell ref="B2:C2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>